<commit_message>
Fix: Corrección de ortografía y fecha en el documento de requerimientos
</commit_message>
<xml_diff>
--- a/doc/Requerimientos funcionales y no funcionales.xlsx
+++ b/doc/Requerimientos funcionales y no funcionales.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A30F0E4-12D6-4FAC-978F-DD8D8BB7E352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31643DB9-CD14-43C9-AD01-685E0CDA8374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de priorización" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
   <si>
-    <t>Última modificación: 30/enero/2025</t>
-  </si>
-  <si>
     <t>Matriz de priorización</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>El sistema permitirá el acceso del usuario por medio de reconocimiento facial</t>
   </si>
   <si>
-    <t>El cliente recibira una alerta de los productos de la tienda que tengan un stock menor a cinco unidades</t>
-  </si>
-  <si>
     <t>El cliente podrá registrar empleados en su gimnasio donde cada uno tendrá un código de acceso</t>
   </si>
   <si>
@@ -184,9 +178,6 @@
     <t>El sistema hará uso de roles y permisos para impedir que los usuarios y empleados entren a las vistas del cliente</t>
   </si>
   <si>
-    <t>El sistema terndrá una respuesta menor a dos segundos para cada página</t>
-  </si>
-  <si>
     <t>El sistema tendrá un diseño responsivo para adaptarse a cualquier pantalla</t>
   </si>
   <si>
@@ -238,13 +229,22 @@
     <t>Descripción</t>
   </si>
   <si>
-    <t>Requisito totalmente impresindible que tiene que estar incluido ya que si no se llevan a acabo el proyecto no puede seguir adelante</t>
-  </si>
-  <si>
     <t>Requisito que debe llevarse a cabo si es posible, es decir, son requisitos importantes y de gran valor para el producto que se está construyendo</t>
   </si>
   <si>
-    <t>Requisitos que podrían incluirse si no afecta a nada más, es decir, son requisitos que sería bueno y podrían inclurise porque no cuesta demasiado implementarlos</t>
+    <t>Fecha: 30/enero/2025</t>
+  </si>
+  <si>
+    <t>El sistema tendrá una respuesta menor a dos segundos para cada página</t>
+  </si>
+  <si>
+    <t>El cliente recibirá una alerta de los productos de la tienda que tengan un stock menor a cinco unidades</t>
+  </si>
+  <si>
+    <t>Requisito totalmente imprescindible que tiene que estar incluido ya que si no se llevan a cabo el proyecto no puede seguir adelante</t>
+  </si>
+  <si>
+    <t>Requisitos que podrían incluirse si no afecta a nada más, es decir, son requisitos que sería bueno y podrían incluirse porque no cuesta demasiado implementarlos</t>
   </si>
 </sst>
 </file>
@@ -786,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F274FABB-DF5C-4F9E-B98F-F8DC866DADF5}">
   <dimension ref="B1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,12 +800,12 @@
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -813,674 +813,674 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="1">
         <v>4</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="1">
         <v>5</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="1">
         <v>5</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1">
         <v>4</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1">
         <v>3</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1">
         <v>4</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="1">
         <v>5</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D26" s="1">
         <v>3</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D27" s="1">
         <v>3</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D29" s="1">
         <v>3</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" s="1">
         <v>3</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1">
         <v>4</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D32" s="1">
         <v>3</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33" s="1">
         <v>4</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D34" s="1">
         <v>3</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D35" s="1">
         <v>5</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D36" s="1">
         <v>5</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D37" s="1">
         <v>4</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D38" s="1">
         <v>5</v>
       </c>
       <c r="E38" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D41" s="1">
         <v>3</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="D43" s="1">
         <v>4</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D46" s="1">
         <v>2</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D47" s="1">
         <v>4</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D48" s="1">
         <v>3</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1">
         <v>4</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -1502,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D8AED2-970B-4AE3-A10B-79DA34B06F7C}">
   <dimension ref="B3:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,42 +1515,42 @@
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="I3" s="12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
         <v>60</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>61</v>
       </c>
-      <c r="D4" t="s">
+      <c r="I4" t="s">
         <v>62</v>
       </c>
-      <c r="E4" t="s">
+      <c r="J4" t="s">
         <v>63</v>
       </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>64</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>66</v>
-      </c>
-      <c r="K4" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1570,25 +1570,25 @@
         <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="I7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="2" t="s">

</xml_diff>

<commit_message>
Doc: Se agregaron nuevos requerimientos y se creó el diagrama de casos de uso
</commit_message>
<xml_diff>
--- a/doc/Requerimientos funcionales y no funcionales.xlsx
+++ b/doc/Requerimientos funcionales y no funcionales.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31643DB9-CD14-43C9-AD01-685E0CDA8374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5621C78A-DCBA-4A86-99E1-485AAB0870FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
+    <workbookView xWindow="13550" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{A22C7B05-6B0A-4116-A99A-60EDDEA67682}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz de priorización" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="72">
   <si>
     <t>Matriz de priorización</t>
   </si>
@@ -67,12 +67,6 @@
     <t>SHOULD</t>
   </si>
   <si>
-    <t>El cliente podrá crear un nuevo gimnasio con nombre, descripción y domicilio</t>
-  </si>
-  <si>
-    <t>El cliente podrá editar un gimnasio creado (nombre, descripción o ubicación)</t>
-  </si>
-  <si>
     <t>El cliente podrá administrar el inventario de las máquinas del gimnasio (crear, actualizar y eliminar).</t>
   </si>
   <si>
@@ -88,12 +82,6 @@
     <t>El cliente podrá administrar al personal del gimnasio (crear, actualizar y eliminar)</t>
   </si>
   <si>
-    <t xml:space="preserve">El cliente podrá generar planes personalizados para que los usuarios se suscriban </t>
-  </si>
-  <si>
-    <t>El cliente tendrá una página personalizada para promocionar su gimnasio con las datos correspondientes (nombre, descripción, ubicación, tienda de productos, máquinas de gimnasio con las que cuentan y planes creados)</t>
-  </si>
-  <si>
     <t>Los usuarios podrán registrarse en la página personalizada del gimnasio del cliente con su correo y una contraseña</t>
   </si>
   <si>
@@ -232,9 +220,6 @@
     <t>Requisito que debe llevarse a cabo si es posible, es decir, son requisitos importantes y de gran valor para el producto que se está construyendo</t>
   </si>
   <si>
-    <t>Fecha: 30/enero/2025</t>
-  </si>
-  <si>
     <t>El sistema tendrá una respuesta menor a dos segundos para cada página</t>
   </si>
   <si>
@@ -245,6 +230,24 @@
   </si>
   <si>
     <t>Requisitos que podrían incluirse si no afecta a nada más, es decir, son requisitos que sería bueno y podrían incluirse porque no cuesta demasiado implementarlos</t>
+  </si>
+  <si>
+    <t>Fecha: 02/febrero/2025</t>
+  </si>
+  <si>
+    <t>El cliente podrá reservarse el derecho de banear a una persona de su gimnasio acorde a las políticas de uso definidas</t>
+  </si>
+  <si>
+    <t>El cliente tendrá una página personalizada para promocionar su gimnasio con los datos correspondientes (nombre, descripción, ubicación, tienda de productos, máquinas de gimnasio con las que cuentan y planes creados)</t>
+  </si>
+  <si>
+    <t>El empleado podrá administrar el inventario de productos en venta (crear, actualizar y eliminar).</t>
+  </si>
+  <si>
+    <t>El cliente podrá administrar gimnasios (crear, actualizar y eliminar).</t>
+  </si>
+  <si>
+    <t>El cliente podrá generar planes personalizados para que los usuarios se suscriban (crear, actualizar y eliminar)</t>
   </si>
 </sst>
 </file>
@@ -429,8 +432,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{558EE57F-5071-4785-8DD6-54905DFB85BB}" name="Tabla2" displayName="Tabla2" ref="B3:E50" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="B3:E50" xr:uid="{558EE57F-5071-4785-8DD6-54905DFB85BB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{558EE57F-5071-4785-8DD6-54905DFB85BB}" name="Tabla2" displayName="Tabla2" ref="B3:E51" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="B3:E51" xr:uid="{558EE57F-5071-4785-8DD6-54905DFB85BB}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{F4186AF0-6301-4943-BE7A-5D40124BB30B}" name="Tipo" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{747A71E2-418C-4C5E-B861-66F3BE066CD9}" name="Requerimiento" dataDxfId="12"/>
@@ -784,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F274FABB-DF5C-4F9E-B98F-F8DC866DADF5}">
-  <dimension ref="B1:E51"/>
+  <dimension ref="B1:E52"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +875,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>70</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
@@ -886,12 +889,12 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -900,13 +903,13 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -914,13 +917,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -928,7 +931,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
@@ -942,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
@@ -951,12 +954,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
@@ -965,26 +968,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E14" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1">
         <v>3</v>
@@ -993,15 +996,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D16" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>7</v>
@@ -1012,27 +1015,27 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1">
-        <v>5</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1">
         <v>5</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -1040,55 +1043,55 @@
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1">
         <v>5</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1">
-        <v>3</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1096,13 +1099,13 @@
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1">
-        <v>4</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1110,13 +1113,13 @@
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D24" s="1">
-        <v>5</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1124,13 +1127,13 @@
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1138,21 +1141,21 @@
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D26" s="1">
-        <v>3</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D27" s="1">
         <v>3</v>
@@ -1161,15 +1164,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>7</v>
@@ -1180,10 +1183,10 @@
         <v>5</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>7</v>
@@ -1194,7 +1197,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D30" s="1">
         <v>3</v>
@@ -1203,60 +1206,60 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D31" s="1">
+        <v>3</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="1">
         <v>4</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E32" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="1">
-        <v>3</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D33" s="1">
+        <v>3</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1">
         <v>4</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="1">
-        <v>3</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1264,13 +1267,13 @@
         <v>5</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D35" s="1">
-        <v>5</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1278,13 +1281,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D36" s="1">
         <v>5</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1292,13 +1295,13 @@
         <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D37" s="1">
-        <v>4</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1306,13 +1309,13 @@
         <v>5</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D38" s="1">
-        <v>5</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -1320,21 +1323,21 @@
         <v>5</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D39" s="1">
-        <v>3</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
@@ -1345,10 +1348,10 @@
     </row>
     <row r="41" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D41" s="1">
         <v>3</v>
@@ -1359,10 +1362,10 @@
     </row>
     <row r="42" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D42" s="1">
         <v>3</v>
@@ -1371,40 +1374,40 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D43" s="1">
-        <v>4</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D44" s="1">
-        <v>3</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
@@ -1415,76 +1418,90 @@
     </row>
     <row r="46" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D46" s="1">
-        <v>2</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D47" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D48" s="1">
-        <v>3</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D49" s="1">
-        <v>4</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D50" s="1">
+        <v>4</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D51" s="1">
         <v>1</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
+      <c r="E51" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1502,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D8AED2-970B-4AE3-A10B-79DA34B06F7C}">
   <dimension ref="B3:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,42 +1532,42 @@
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="I3" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
         <v>59</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>60</v>
-      </c>
-      <c r="F4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1574,7 +1591,7 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="30" x14ac:dyDescent="0.25">
@@ -1583,16 +1600,16 @@
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="I7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>